<commit_message>
added animal_type column to animal.xls
</commit_message>
<xml_diff>
--- a/Excel/Animal.xlsx
+++ b/Excel/Animal.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
   <si>
     <t>ID</t>
   </si>
@@ -73,6 +73,9 @@
     <t>物件类型</t>
   </si>
   <si>
+    <t>动物种类</t>
+  </si>
+  <si>
     <t>成长时间</t>
   </si>
   <si>
@@ -97,6 +100,9 @@
     <t>farm_type</t>
   </si>
   <si>
+    <t>animal_type</t>
+  </si>
+  <si>
     <t>time_min</t>
   </si>
   <si>
@@ -115,7 +121,7 @@
     <t>string</t>
   </si>
   <si>
-    <t>1011</t>
+    <t>2011</t>
   </si>
   <si>
     <t>AnimalChicken_01</t>
@@ -127,16 +133,16 @@
     <t>2</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>60</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
-    <t>1012</t>
+    <t>2012</t>
   </si>
   <si>
     <t>AnimalChicken_02</t>
@@ -148,7 +154,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>1021</t>
+    <t>2021</t>
   </si>
   <si>
     <t>AnimalGoose_01</t>
@@ -163,7 +169,7 @@
     <t>12</t>
   </si>
   <si>
-    <t>1022</t>
+    <t>2022</t>
   </si>
   <si>
     <t>AnimalGoose_02</t>
@@ -172,7 +178,7 @@
     <t>鹅_成年</t>
   </si>
   <si>
-    <t>1031</t>
+    <t>2031</t>
   </si>
   <si>
     <t>AnimalSheep_01</t>
@@ -181,13 +187,16 @@
     <t>羊_幼年</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>180</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>1032</t>
+    <t>2032</t>
   </si>
   <si>
     <t>AnimalSheep_02</t>
@@ -196,7 +205,7 @@
     <t>羊_成年</t>
   </si>
   <si>
-    <t>1041</t>
+    <t>2041</t>
   </si>
   <si>
     <t>AnimalCattle_01</t>
@@ -205,16 +214,16 @@
     <t>牛_幼年</t>
   </si>
   <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>240</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>5</t>
   </si>
   <si>
-    <t>1042</t>
+    <t>2042</t>
   </si>
   <si>
     <t>AnimalCattle_02</t>
@@ -223,7 +232,7 @@
     <t>牛_成年</t>
   </si>
   <si>
-    <t>1051</t>
+    <t>2051</t>
   </si>
   <si>
     <t>AnimalPig_01</t>
@@ -238,7 +247,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>1052</t>
+    <t>2052</t>
   </si>
   <si>
     <t>AnimalPig_02</t>
@@ -247,7 +256,7 @@
     <t>猪_成年</t>
   </si>
   <si>
-    <t>1061</t>
+    <t>2061</t>
   </si>
   <si>
     <t>AnimalHorse_01</t>
@@ -259,10 +268,7 @@
     <t>480</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>1062</t>
+    <t>2062</t>
   </si>
   <si>
     <t>AnimalHorse_02</t>
@@ -434,12 +440,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1226,23 +1232,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="19.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.125" style="1" customWidth="1"/>
-    <col min="4" max="7" width="18.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="4" max="8" width="18.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" ht="26" customHeight="1" spans="1:8">
+    <row r="1" customFormat="1" ht="26" customHeight="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1267,103 +1273,115 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" spans="1:8">
+    <row r="2" customFormat="1" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" customFormat="1" spans="1:8">
+    <row r="3" customFormat="1" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:8">
+    <row r="4" customFormat="1" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:8">
+    <row r="5" customFormat="1" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>24</v>
@@ -1371,265 +1389,298 @@
       <c r="H5" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" customFormat="1" spans="1:8">
+    <row r="6" customFormat="1" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" customFormat="1" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="8" customFormat="1" spans="1:8">
+    <row r="8" customFormat="1" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="9" customFormat="1" spans="1:8">
+    <row r="9" customFormat="1" spans="1:9">
       <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>43</v>
+      <c r="I9" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="10" customFormat="1" spans="1:8">
+    <row r="10" customFormat="1" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="11" customFormat="1" spans="1:8">
+    <row r="11" customFormat="1" spans="1:9">
       <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>52</v>
+      <c r="I11" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="12" customFormat="1" spans="1:8">
+    <row r="12" customFormat="1" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
+        <v>23</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="13" customFormat="1" spans="1:8">
+    <row r="13" customFormat="1" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>60</v>
+      <c r="I13" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="1:8">
+    <row r="14" customFormat="1" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>63</v>
-      </c>
     </row>
-    <row r="15" customFormat="1" spans="1:8">
+    <row r="15" customFormat="1" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added harvest_item_id in animal.xls
</commit_message>
<xml_diff>
--- a/Excel/Animal.xlsx
+++ b/Excel/Animal.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -79,6 +79,9 @@
     <t>成长时间</t>
   </si>
   <si>
+    <t>收获物品</t>
+  </si>
+  <si>
     <t>等级需求</t>
   </si>
   <si>
@@ -106,6 +109,9 @@
     <t>time_min</t>
   </si>
   <si>
+    <t>harvest_item_id</t>
+  </si>
+  <si>
     <t>level_need</t>
   </si>
   <si>
@@ -154,6 +160,9 @@
     <t>0</t>
   </si>
   <si>
+    <t>300101</t>
+  </si>
+  <si>
     <t>2021</t>
   </si>
   <si>
@@ -178,6 +187,9 @@
     <t>鹅_成年</t>
   </si>
   <si>
+    <t>300102</t>
+  </si>
+  <si>
     <t>2031</t>
   </si>
   <si>
@@ -205,6 +217,9 @@
     <t>羊_成年</t>
   </si>
   <si>
+    <t>300103</t>
+  </si>
+  <si>
     <t>2041</t>
   </si>
   <si>
@@ -232,6 +247,9 @@
     <t>牛_成年</t>
   </si>
   <si>
+    <t>300104</t>
+  </si>
+  <si>
     <t>2051</t>
   </si>
   <si>
@@ -256,6 +274,9 @@
     <t>猪_成年</t>
   </si>
   <si>
+    <t>300105</t>
+  </si>
+  <si>
     <t>2061</t>
   </si>
   <si>
@@ -275,6 +296,9 @@
   </si>
   <si>
     <t>马_成年</t>
+  </si>
+  <si>
+    <t>300106</t>
   </si>
 </sst>
 </file>
@@ -440,12 +464,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1232,10 +1256,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -1243,12 +1267,12 @@
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="2" width="19.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.125" style="1" customWidth="1"/>
-    <col min="4" max="8" width="18.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9" style="1"/>
+    <col min="4" max="9" width="18.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" ht="26" customHeight="1" spans="1:9">
+    <row r="1" customFormat="1" ht="26" customHeight="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1276,115 +1300,125 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" spans="1:9">
+    <row r="2" customFormat="1" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" customFormat="1" spans="1:9">
+    <row r="3" customFormat="1" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="1" spans="1:9">
+    <row r="4" customFormat="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="5" customFormat="1" spans="1:9">
+    <row r="5" customFormat="1" spans="1:10">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>26</v>
@@ -1392,295 +1426,318 @@
       <c r="I5" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="6" customFormat="1" spans="1:9">
+    <row r="6" customFormat="1" spans="1:10">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" spans="1:10">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" spans="1:10">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:10">
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" customFormat="1" spans="1:9">
-      <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>37</v>
+    <row r="10" customFormat="1" spans="1:10">
+      <c r="A10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="8" customFormat="1" spans="1:9">
-      <c r="A8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>40</v>
+    <row r="11" customFormat="1" spans="1:10">
+      <c r="A11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="9" customFormat="1" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="12" customFormat="1" spans="1:10">
+      <c r="A12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" s="1" t="s">
+      <c r="I12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" spans="1:10">
+      <c r="A13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="10" customFormat="1" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>49</v>
+    <row r="14" customFormat="1" spans="1:10">
+      <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="11" customFormat="1" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="4" t="s">
+    <row r="15" customFormat="1" spans="1:10">
+      <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" customFormat="1" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" customFormat="1" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" customFormat="1" spans="1:9">
-      <c r="A15" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="I15" s="1" t="s">
-        <v>70</v>
+        <v>46</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>